<commit_message>
Changed the data "days" instead of being the days of life (from when they were sown, I put the treatment period days). This mainly because the 2 species were sown in different dates.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Desktop\Mari\UPV\Climate change\R greenhouse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carolina Junca\Documents\Greenhouse-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B0C45F-F733-4D5F-A9C8-CB37DEA15BBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="17556" yWindow="6144" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -301,7 +302,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -578,17 +579,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="E229" sqref="E229"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" customWidth="1"/>
     <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -627,7 +629,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2">
         <v>3</v>
@@ -653,7 +655,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
         <v>4</v>
@@ -679,7 +681,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <v>4</v>
@@ -705,7 +707,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2">
         <v>3</v>
@@ -731,7 +733,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <v>4</v>
@@ -757,7 +759,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2">
         <v>3</v>
@@ -783,7 +785,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D8" s="3">
         <v>3</v>
@@ -809,7 +811,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D9" s="3">
         <v>3</v>
@@ -835,7 +837,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D10" s="3">
         <v>3</v>
@@ -861,7 +863,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D11" s="3">
         <v>3</v>
@@ -887,7 +889,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D12" s="3">
         <v>3</v>
@@ -913,7 +915,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D13" s="3">
         <v>3</v>
@@ -939,7 +941,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2">
         <v>3</v>
@@ -965,7 +967,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2">
         <v>3</v>
@@ -991,7 +993,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
@@ -1017,7 +1019,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2">
         <v>3</v>
@@ -1043,7 +1045,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2">
         <v>4</v>
@@ -1069,7 +1071,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2">
         <v>4</v>
@@ -1095,7 +1097,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D20" s="3">
         <v>3</v>
@@ -1121,7 +1123,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D21" s="3">
         <v>4</v>
@@ -1147,7 +1149,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D22" s="3">
         <v>4</v>
@@ -1173,7 +1175,7 @@
         <v>7</v>
       </c>
       <c r="C23" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D23" s="3">
         <v>3</v>
@@ -1199,7 +1201,7 @@
         <v>7</v>
       </c>
       <c r="C24" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D24" s="3">
         <v>3</v>
@@ -1225,7 +1227,7 @@
         <v>7</v>
       </c>
       <c r="C25" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D25" s="3">
         <v>3</v>
@@ -1251,7 +1253,7 @@
         <v>8</v>
       </c>
       <c r="C26" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2">
         <v>2</v>
@@ -1277,7 +1279,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
@@ -1303,7 +1305,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D28" s="2">
         <v>2</v>
@@ -1329,7 +1331,7 @@
         <v>8</v>
       </c>
       <c r="C29" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
@@ -1355,7 +1357,7 @@
         <v>8</v>
       </c>
       <c r="C30" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D30" s="2">
         <v>2</v>
@@ -1381,7 +1383,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D31" s="2">
         <v>2</v>
@@ -1407,7 +1409,7 @@
         <v>8</v>
       </c>
       <c r="C32" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D32" s="3">
         <v>2</v>
@@ -1433,7 +1435,7 @@
         <v>8</v>
       </c>
       <c r="C33" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D33" s="3">
         <v>2</v>
@@ -1459,7 +1461,7 @@
         <v>8</v>
       </c>
       <c r="C34" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D34" s="3">
         <v>2</v>
@@ -1485,7 +1487,7 @@
         <v>8</v>
       </c>
       <c r="C35" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D35" s="3">
         <v>2</v>
@@ -1511,7 +1513,7 @@
         <v>8</v>
       </c>
       <c r="C36" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D36" s="3">
         <v>2</v>
@@ -1537,7 +1539,7 @@
         <v>8</v>
       </c>
       <c r="C37" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D37" s="3">
         <v>2</v>
@@ -1563,7 +1565,7 @@
         <v>8</v>
       </c>
       <c r="C38" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D38" s="2">
         <v>2</v>
@@ -1589,7 +1591,7 @@
         <v>8</v>
       </c>
       <c r="C39" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D39" s="2">
         <v>2</v>
@@ -1615,7 +1617,7 @@
         <v>8</v>
       </c>
       <c r="C40" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D40" s="2">
         <v>2</v>
@@ -1641,7 +1643,7 @@
         <v>8</v>
       </c>
       <c r="C41" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -1667,7 +1669,7 @@
         <v>8</v>
       </c>
       <c r="C42" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D42" s="2">
         <v>2</v>
@@ -1693,7 +1695,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D43" s="2">
         <v>2</v>
@@ -1719,7 +1721,7 @@
         <v>8</v>
       </c>
       <c r="C44" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D44" s="3">
         <v>2</v>
@@ -1745,7 +1747,7 @@
         <v>8</v>
       </c>
       <c r="C45" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D45" s="3">
         <v>2</v>
@@ -1771,7 +1773,7 @@
         <v>8</v>
       </c>
       <c r="C46" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D46" s="3">
         <v>1</v>
@@ -1797,7 +1799,7 @@
         <v>8</v>
       </c>
       <c r="C47" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D47" s="3">
         <v>2</v>
@@ -1823,7 +1825,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D48" s="3">
         <v>2</v>
@@ -1849,7 +1851,7 @@
         <v>8</v>
       </c>
       <c r="C49" s="17">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D49" s="4">
         <v>2</v>
@@ -1875,7 +1877,7 @@
         <v>7</v>
       </c>
       <c r="C50" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D50" s="5">
         <v>4</v>
@@ -1901,7 +1903,7 @@
         <v>7</v>
       </c>
       <c r="C51" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D51" s="5">
         <v>4</v>
@@ -1927,7 +1929,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D52" s="5">
         <v>5</v>
@@ -1953,7 +1955,7 @@
         <v>7</v>
       </c>
       <c r="C53" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D53" s="5">
         <v>4</v>
@@ -1979,7 +1981,7 @@
         <v>7</v>
       </c>
       <c r="C54" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D54" s="5">
         <v>4</v>
@@ -2005,7 +2007,7 @@
         <v>7</v>
       </c>
       <c r="C55" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D55" s="5">
         <v>5</v>
@@ -2031,7 +2033,7 @@
         <v>7</v>
       </c>
       <c r="C56" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D56" s="6">
         <v>4</v>
@@ -2057,7 +2059,7 @@
         <v>7</v>
       </c>
       <c r="C57" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D57" s="6">
         <v>4</v>
@@ -2083,7 +2085,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D58" s="6">
         <v>4</v>
@@ -2109,7 +2111,7 @@
         <v>7</v>
       </c>
       <c r="C59" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D59" s="6">
         <v>4</v>
@@ -2135,7 +2137,7 @@
         <v>7</v>
       </c>
       <c r="C60" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D60" s="6">
         <v>4</v>
@@ -2161,7 +2163,7 @@
         <v>7</v>
       </c>
       <c r="C61" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D61" s="6">
         <v>5</v>
@@ -2187,7 +2189,7 @@
         <v>7</v>
       </c>
       <c r="C62" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D62" s="5">
         <v>5</v>
@@ -2213,7 +2215,7 @@
         <v>7</v>
       </c>
       <c r="C63" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D63" s="5">
         <v>4</v>
@@ -2239,7 +2241,7 @@
         <v>7</v>
       </c>
       <c r="C64" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D64" s="5">
         <v>4</v>
@@ -2265,7 +2267,7 @@
         <v>7</v>
       </c>
       <c r="C65" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D65" s="5">
         <v>4</v>
@@ -2291,7 +2293,7 @@
         <v>7</v>
       </c>
       <c r="C66" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D66" s="5">
         <v>5</v>
@@ -2317,7 +2319,7 @@
         <v>7</v>
       </c>
       <c r="C67" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D67" s="5">
         <v>4</v>
@@ -2343,7 +2345,7 @@
         <v>7</v>
       </c>
       <c r="C68" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D68" s="6">
         <v>4</v>
@@ -2369,7 +2371,7 @@
         <v>7</v>
       </c>
       <c r="C69" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D69" s="6">
         <v>5</v>
@@ -2395,7 +2397,7 @@
         <v>7</v>
       </c>
       <c r="C70" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D70" s="6">
         <v>4</v>
@@ -2421,7 +2423,7 @@
         <v>7</v>
       </c>
       <c r="C71" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D71" s="6">
         <v>4</v>
@@ -2447,7 +2449,7 @@
         <v>7</v>
       </c>
       <c r="C72" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D72" s="6">
         <v>4</v>
@@ -2473,7 +2475,7 @@
         <v>7</v>
       </c>
       <c r="C73" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D73" s="6">
         <v>4</v>
@@ -2499,7 +2501,7 @@
         <v>8</v>
       </c>
       <c r="C74" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D74" s="5">
         <v>2</v>
@@ -2525,7 +2527,7 @@
         <v>8</v>
       </c>
       <c r="C75" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D75" s="5">
         <v>2</v>
@@ -2551,7 +2553,7 @@
         <v>8</v>
       </c>
       <c r="C76" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D76" s="5">
         <v>2</v>
@@ -2577,7 +2579,7 @@
         <v>8</v>
       </c>
       <c r="C77" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D77" s="5">
         <v>2</v>
@@ -2603,7 +2605,7 @@
         <v>8</v>
       </c>
       <c r="C78" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D78" s="5">
         <v>2</v>
@@ -2629,7 +2631,7 @@
         <v>8</v>
       </c>
       <c r="C79" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D79" s="5">
         <v>2</v>
@@ -2655,7 +2657,7 @@
         <v>8</v>
       </c>
       <c r="C80" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D80" s="6">
         <v>2</v>
@@ -2681,7 +2683,7 @@
         <v>8</v>
       </c>
       <c r="C81" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D81" s="6">
         <v>3</v>
@@ -2707,7 +2709,7 @@
         <v>8</v>
       </c>
       <c r="C82" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D82" s="6">
         <v>2</v>
@@ -2733,7 +2735,7 @@
         <v>8</v>
       </c>
       <c r="C83" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D83" s="6">
         <v>2</v>
@@ -2759,7 +2761,7 @@
         <v>8</v>
       </c>
       <c r="C84" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D84" s="6">
         <v>2</v>
@@ -2785,7 +2787,7 @@
         <v>8</v>
       </c>
       <c r="C85" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D85" s="6">
         <v>2</v>
@@ -2811,7 +2813,7 @@
         <v>8</v>
       </c>
       <c r="C86" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D86" s="5">
         <v>2</v>
@@ -2837,7 +2839,7 @@
         <v>8</v>
       </c>
       <c r="C87" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D87" s="5">
         <v>2</v>
@@ -2863,7 +2865,7 @@
         <v>8</v>
       </c>
       <c r="C88" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D88" s="5">
         <v>2</v>
@@ -2889,7 +2891,7 @@
         <v>8</v>
       </c>
       <c r="C89" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D89" s="5">
         <v>2</v>
@@ -2915,7 +2917,7 @@
         <v>8</v>
       </c>
       <c r="C90" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D90" s="5">
         <v>3</v>
@@ -2941,7 +2943,7 @@
         <v>8</v>
       </c>
       <c r="C91" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D91" s="5">
         <v>2</v>
@@ -2967,7 +2969,7 @@
         <v>8</v>
       </c>
       <c r="C92" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D92" s="6">
         <v>3</v>
@@ -2993,7 +2995,7 @@
         <v>8</v>
       </c>
       <c r="C93" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D93" s="6">
         <v>2</v>
@@ -3019,7 +3021,7 @@
         <v>8</v>
       </c>
       <c r="C94" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D94" s="6">
         <v>2</v>
@@ -3045,7 +3047,7 @@
         <v>8</v>
       </c>
       <c r="C95" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D95" s="6">
         <v>2</v>
@@ -3071,7 +3073,7 @@
         <v>8</v>
       </c>
       <c r="C96" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D96" s="6">
         <v>2</v>
@@ -3097,7 +3099,7 @@
         <v>8</v>
       </c>
       <c r="C97" s="17">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D97" s="7">
         <v>2</v>
@@ -3123,7 +3125,7 @@
         <v>7</v>
       </c>
       <c r="C98" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D98" s="5">
         <v>4</v>
@@ -3149,7 +3151,7 @@
         <v>7</v>
       </c>
       <c r="C99" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D99" s="5">
         <v>5</v>
@@ -3175,7 +3177,7 @@
         <v>7</v>
       </c>
       <c r="C100" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D100" s="5">
         <v>6</v>
@@ -3201,7 +3203,7 @@
         <v>7</v>
       </c>
       <c r="C101" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D101" s="5">
         <v>4</v>
@@ -3227,7 +3229,7 @@
         <v>7</v>
       </c>
       <c r="C102" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D102" s="5">
         <v>5</v>
@@ -3253,7 +3255,7 @@
         <v>7</v>
       </c>
       <c r="C103" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D103" s="5">
         <v>7</v>
@@ -3279,7 +3281,7 @@
         <v>7</v>
       </c>
       <c r="C104" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D104" s="6">
         <v>4</v>
@@ -3305,7 +3307,7 @@
         <v>7</v>
       </c>
       <c r="C105" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D105" s="6">
         <v>4</v>
@@ -3331,7 +3333,7 @@
         <v>7</v>
       </c>
       <c r="C106" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D106" s="6">
         <v>4</v>
@@ -3357,7 +3359,7 @@
         <v>7</v>
       </c>
       <c r="C107" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D107" s="6">
         <v>4</v>
@@ -3383,7 +3385,7 @@
         <v>7</v>
       </c>
       <c r="C108" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D108" s="6">
         <v>4</v>
@@ -3409,7 +3411,7 @@
         <v>7</v>
       </c>
       <c r="C109" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D109" s="6">
         <v>5</v>
@@ -3435,7 +3437,7 @@
         <v>7</v>
       </c>
       <c r="C110" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D110" s="5">
         <v>6</v>
@@ -3461,7 +3463,7 @@
         <v>7</v>
       </c>
       <c r="C111" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D111" s="5">
         <v>5</v>
@@ -3487,7 +3489,7 @@
         <v>7</v>
       </c>
       <c r="C112" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D112" s="5">
         <v>5</v>
@@ -3513,7 +3515,7 @@
         <v>7</v>
       </c>
       <c r="C113" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D113" s="5">
         <v>5</v>
@@ -3539,7 +3541,7 @@
         <v>7</v>
       </c>
       <c r="C114" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D114" s="5">
         <v>5</v>
@@ -3565,7 +3567,7 @@
         <v>7</v>
       </c>
       <c r="C115" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D115" s="5">
         <v>5</v>
@@ -3591,7 +3593,7 @@
         <v>7</v>
       </c>
       <c r="C116" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D116" s="6">
         <v>4</v>
@@ -3617,7 +3619,7 @@
         <v>7</v>
       </c>
       <c r="C117" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D117" s="6">
         <v>5</v>
@@ -3643,7 +3645,7 @@
         <v>7</v>
       </c>
       <c r="C118" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D118" s="6">
         <v>5</v>
@@ -3669,7 +3671,7 @@
         <v>7</v>
       </c>
       <c r="C119" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D119" s="6">
         <v>6</v>
@@ -3695,7 +3697,7 @@
         <v>7</v>
       </c>
       <c r="C120" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D120" s="6">
         <v>4</v>
@@ -3721,7 +3723,7 @@
         <v>7</v>
       </c>
       <c r="C121" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D121" s="6">
         <v>5</v>
@@ -3747,7 +3749,7 @@
         <v>8</v>
       </c>
       <c r="C122" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D122" s="5">
         <v>3</v>
@@ -3773,7 +3775,7 @@
         <v>8</v>
       </c>
       <c r="C123" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D123" s="5">
         <v>3</v>
@@ -3799,7 +3801,7 @@
         <v>8</v>
       </c>
       <c r="C124" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D124" s="5">
         <v>3</v>
@@ -3825,7 +3827,7 @@
         <v>8</v>
       </c>
       <c r="C125" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D125" s="5">
         <v>3</v>
@@ -3851,7 +3853,7 @@
         <v>8</v>
       </c>
       <c r="C126" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D126" s="5">
         <v>2</v>
@@ -3877,7 +3879,7 @@
         <v>8</v>
       </c>
       <c r="C127" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D127" s="5">
         <v>3</v>
@@ -3903,7 +3905,7 @@
         <v>8</v>
       </c>
       <c r="C128" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D128" s="6">
         <v>3</v>
@@ -3929,7 +3931,7 @@
         <v>8</v>
       </c>
       <c r="C129" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D129" s="6">
         <v>3</v>
@@ -3955,7 +3957,7 @@
         <v>8</v>
       </c>
       <c r="C130" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D130" s="6">
         <v>3</v>
@@ -3981,7 +3983,7 @@
         <v>8</v>
       </c>
       <c r="C131" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D131" s="6">
         <v>3</v>
@@ -4007,7 +4009,7 @@
         <v>8</v>
       </c>
       <c r="C132" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D132" s="6">
         <v>2</v>
@@ -4033,7 +4035,7 @@
         <v>8</v>
       </c>
       <c r="C133" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D133" s="6">
         <v>3</v>
@@ -4059,7 +4061,7 @@
         <v>8</v>
       </c>
       <c r="C134" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D134" s="5">
         <v>2</v>
@@ -4085,7 +4087,7 @@
         <v>8</v>
       </c>
       <c r="C135" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D135" s="5">
         <v>2</v>
@@ -4111,7 +4113,7 @@
         <v>8</v>
       </c>
       <c r="C136" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D136" s="5">
         <v>3</v>
@@ -4137,7 +4139,7 @@
         <v>8</v>
       </c>
       <c r="C137" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D137" s="5">
         <v>2</v>
@@ -4163,7 +4165,7 @@
         <v>8</v>
       </c>
       <c r="C138" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D138" s="5">
         <v>4</v>
@@ -4189,7 +4191,7 @@
         <v>8</v>
       </c>
       <c r="C139" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D139" s="5">
         <v>2</v>
@@ -4215,7 +4217,7 @@
         <v>8</v>
       </c>
       <c r="C140" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D140" s="6">
         <v>4</v>
@@ -4241,7 +4243,7 @@
         <v>8</v>
       </c>
       <c r="C141" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D141" s="6">
         <v>2</v>
@@ -4267,7 +4269,7 @@
         <v>8</v>
       </c>
       <c r="C142" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D142" s="6">
         <v>3</v>
@@ -4293,7 +4295,7 @@
         <v>8</v>
       </c>
       <c r="C143" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D143" s="6">
         <v>3</v>
@@ -4319,7 +4321,7 @@
         <v>8</v>
       </c>
       <c r="C144" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D144" s="6">
         <v>3</v>
@@ -4345,7 +4347,7 @@
         <v>8</v>
       </c>
       <c r="C145" s="17">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D145" s="6">
         <v>3</v>
@@ -4371,7 +4373,7 @@
         <v>7</v>
       </c>
       <c r="C146" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D146" s="8">
         <v>5</v>
@@ -4397,7 +4399,7 @@
         <v>7</v>
       </c>
       <c r="C147" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D147" s="5">
         <v>7</v>
@@ -4423,7 +4425,7 @@
         <v>7</v>
       </c>
       <c r="C148" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D148" s="5">
         <v>7</v>
@@ -4449,7 +4451,7 @@
         <v>7</v>
       </c>
       <c r="C149" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D149" s="5">
         <v>6</v>
@@ -4475,7 +4477,7 @@
         <v>7</v>
       </c>
       <c r="C150" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D150" s="5">
         <v>6</v>
@@ -4501,7 +4503,7 @@
         <v>7</v>
       </c>
       <c r="C151" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D151" s="5">
         <v>10</v>
@@ -4527,7 +4529,7 @@
         <v>7</v>
       </c>
       <c r="C152" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D152" s="9">
         <v>4</v>
@@ -4551,7 +4553,7 @@
         <v>7</v>
       </c>
       <c r="C153" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D153" s="9">
         <v>5</v>
@@ -4575,7 +4577,7 @@
         <v>7</v>
       </c>
       <c r="C154" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D154" s="9">
         <v>5</v>
@@ -4599,7 +4601,7 @@
         <v>7</v>
       </c>
       <c r="C155" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D155" s="9">
         <v>4</v>
@@ -4623,7 +4625,7 @@
         <v>7</v>
       </c>
       <c r="C156" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D156" s="9">
         <v>5</v>
@@ -4647,7 +4649,7 @@
         <v>7</v>
       </c>
       <c r="C157" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D157" s="9">
         <v>6</v>
@@ -4671,7 +4673,7 @@
         <v>7</v>
       </c>
       <c r="C158" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D158" s="5">
         <v>7</v>
@@ -4697,7 +4699,7 @@
         <v>7</v>
       </c>
       <c r="C159" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D159" s="5">
         <v>7</v>
@@ -4723,7 +4725,7 @@
         <v>7</v>
       </c>
       <c r="C160" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D160" s="5">
         <v>6</v>
@@ -4749,7 +4751,7 @@
         <v>7</v>
       </c>
       <c r="C161" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D161" s="5">
         <v>6</v>
@@ -4775,7 +4777,7 @@
         <v>7</v>
       </c>
       <c r="C162" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D162" s="5">
         <v>6</v>
@@ -4801,7 +4803,7 @@
         <v>7</v>
       </c>
       <c r="C163" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D163" s="5">
         <v>6</v>
@@ -4827,7 +4829,7 @@
         <v>7</v>
       </c>
       <c r="C164" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D164" s="6">
         <v>5</v>
@@ -4853,7 +4855,7 @@
         <v>7</v>
       </c>
       <c r="C165" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D165" s="6">
         <v>7</v>
@@ -4879,7 +4881,7 @@
         <v>7</v>
       </c>
       <c r="C166" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D166" s="6">
         <v>6</v>
@@ -4905,7 +4907,7 @@
         <v>7</v>
       </c>
       <c r="C167" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D167" s="6">
         <v>7</v>
@@ -4931,7 +4933,7 @@
         <v>7</v>
       </c>
       <c r="C168" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D168" s="6">
         <v>6</v>
@@ -4957,7 +4959,7 @@
         <v>7</v>
       </c>
       <c r="C169" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D169" s="6">
         <v>6</v>
@@ -4983,7 +4985,7 @@
         <v>8</v>
       </c>
       <c r="C170" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D170" s="5">
         <v>3</v>
@@ -5009,7 +5011,7 @@
         <v>8</v>
       </c>
       <c r="C171" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D171" s="5">
         <v>2</v>
@@ -5035,7 +5037,7 @@
         <v>8</v>
       </c>
       <c r="C172" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D172" s="5">
         <v>4</v>
@@ -5061,7 +5063,7 @@
         <v>8</v>
       </c>
       <c r="C173" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D173" s="5">
         <v>4</v>
@@ -5087,7 +5089,7 @@
         <v>8</v>
       </c>
       <c r="C174" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D174" s="5">
         <v>3</v>
@@ -5113,7 +5115,7 @@
         <v>8</v>
       </c>
       <c r="C175" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D175" s="5">
         <v>4</v>
@@ -5139,7 +5141,7 @@
         <v>8</v>
       </c>
       <c r="C176" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D176" s="6">
         <v>2</v>
@@ -5165,7 +5167,7 @@
         <v>8</v>
       </c>
       <c r="C177" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D177" s="6">
         <v>2</v>
@@ -5191,7 +5193,7 @@
         <v>8</v>
       </c>
       <c r="C178" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D178" s="6">
         <v>2</v>
@@ -5217,7 +5219,7 @@
         <v>8</v>
       </c>
       <c r="C179" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D179" s="6">
         <v>2</v>
@@ -5243,7 +5245,7 @@
         <v>8</v>
       </c>
       <c r="C180" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D180" s="6">
         <v>2</v>
@@ -5269,7 +5271,7 @@
         <v>8</v>
       </c>
       <c r="C181" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D181" s="6">
         <v>2</v>
@@ -5295,7 +5297,7 @@
         <v>8</v>
       </c>
       <c r="C182" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D182" s="5">
         <v>2</v>
@@ -5317,7 +5319,7 @@
         <v>8</v>
       </c>
       <c r="C183" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D183" s="5">
         <v>2</v>
@@ -5343,7 +5345,7 @@
         <v>8</v>
       </c>
       <c r="C184" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D184" s="5">
         <v>3</v>
@@ -5365,7 +5367,7 @@
         <v>8</v>
       </c>
       <c r="C185" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D185" s="5">
         <v>3</v>
@@ -5387,7 +5389,7 @@
         <v>8</v>
       </c>
       <c r="C186" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D186" s="5">
         <v>3</v>
@@ -5409,7 +5411,7 @@
         <v>8</v>
       </c>
       <c r="C187" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D187" s="5">
         <v>1</v>
@@ -5431,7 +5433,7 @@
         <v>8</v>
       </c>
       <c r="C188" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D188" s="6">
         <v>3</v>
@@ -5457,7 +5459,7 @@
         <v>8</v>
       </c>
       <c r="C189" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D189" s="6">
         <v>2</v>
@@ -5483,7 +5485,7 @@
         <v>8</v>
       </c>
       <c r="C190" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D190" s="6">
         <v>3</v>
@@ -5505,7 +5507,7 @@
         <v>8</v>
       </c>
       <c r="C191" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D191" s="6">
         <v>3</v>
@@ -5527,7 +5529,7 @@
         <v>8</v>
       </c>
       <c r="C192" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D192" s="6">
         <v>3</v>
@@ -5551,7 +5553,7 @@
         <v>8</v>
       </c>
       <c r="C193" s="18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D193" s="7">
         <v>2</v>
@@ -5573,7 +5575,7 @@
         <v>7</v>
       </c>
       <c r="C194" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D194" s="8">
         <v>6</v>
@@ -5599,7 +5601,7 @@
         <v>7</v>
       </c>
       <c r="C195" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D195" s="5">
         <v>8</v>
@@ -5625,7 +5627,7 @@
         <v>7</v>
       </c>
       <c r="C196" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D196" s="5">
         <v>8</v>
@@ -5651,7 +5653,7 @@
         <v>7</v>
       </c>
       <c r="C197" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D197" s="5">
         <v>8</v>
@@ -5677,7 +5679,7 @@
         <v>7</v>
       </c>
       <c r="C198" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D198" s="5">
         <v>7</v>
@@ -5703,7 +5705,7 @@
         <v>7</v>
       </c>
       <c r="C199" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D199" s="5">
         <v>11</v>
@@ -5729,7 +5731,7 @@
         <v>7</v>
       </c>
       <c r="C200" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D200" s="12">
         <v>0</v>
@@ -5751,7 +5753,7 @@
         <v>7</v>
       </c>
       <c r="C201" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D201" s="12">
         <v>0</v>
@@ -5773,7 +5775,7 @@
         <v>7</v>
       </c>
       <c r="C202" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D202" s="12">
         <v>0</v>
@@ -5795,7 +5797,7 @@
         <v>7</v>
       </c>
       <c r="C203" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D203" s="12">
         <v>0</v>
@@ -5817,7 +5819,7 @@
         <v>7</v>
       </c>
       <c r="C204" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D204" s="12">
         <v>0</v>
@@ -5839,7 +5841,7 @@
         <v>7</v>
       </c>
       <c r="C205" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D205" s="12">
         <v>0</v>
@@ -5861,7 +5863,7 @@
         <v>7</v>
       </c>
       <c r="C206" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D206" s="5">
         <v>6</v>
@@ -5887,7 +5889,7 @@
         <v>7</v>
       </c>
       <c r="C207" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D207" s="5">
         <v>7</v>
@@ -5913,7 +5915,7 @@
         <v>7</v>
       </c>
       <c r="C208" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D208" s="5">
         <v>6</v>
@@ -5939,7 +5941,7 @@
         <v>7</v>
       </c>
       <c r="C209" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D209" s="5">
         <v>7</v>
@@ -5965,7 +5967,7 @@
         <v>7</v>
       </c>
       <c r="C210" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D210" s="5">
         <v>3</v>
@@ -5991,7 +5993,7 @@
         <v>7</v>
       </c>
       <c r="C211" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D211" s="5">
         <v>5</v>
@@ -6017,7 +6019,7 @@
         <v>7</v>
       </c>
       <c r="C212" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D212" s="6">
         <v>5</v>
@@ -6043,7 +6045,7 @@
         <v>7</v>
       </c>
       <c r="C213" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D213" s="6">
         <v>7</v>
@@ -6065,7 +6067,7 @@
         <v>7</v>
       </c>
       <c r="C214" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D214" s="6">
         <v>5</v>
@@ -6091,7 +6093,7 @@
         <v>7</v>
       </c>
       <c r="C215" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D215" s="6">
         <v>5</v>
@@ -6113,7 +6115,7 @@
         <v>7</v>
       </c>
       <c r="C216" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D216" s="6">
         <v>6</v>
@@ -6139,7 +6141,7 @@
         <v>7</v>
       </c>
       <c r="C217" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D217" s="6">
         <v>6</v>
@@ -6161,7 +6163,7 @@
         <v>8</v>
       </c>
       <c r="C218" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D218" s="5">
         <v>4</v>
@@ -6187,7 +6189,7 @@
         <v>8</v>
       </c>
       <c r="C219" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D219" s="5">
         <v>4</v>
@@ -6213,7 +6215,7 @@
         <v>8</v>
       </c>
       <c r="C220" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D220" s="5">
         <v>5</v>
@@ -6239,7 +6241,7 @@
         <v>8</v>
       </c>
       <c r="C221" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D221" s="5">
         <v>5</v>
@@ -6265,7 +6267,7 @@
         <v>8</v>
       </c>
       <c r="C222" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D222" s="5">
         <v>4</v>
@@ -6291,7 +6293,7 @@
         <v>8</v>
       </c>
       <c r="C223" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D223" s="5">
         <v>5</v>
@@ -6317,7 +6319,7 @@
         <v>8</v>
       </c>
       <c r="C224" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D224" s="6">
         <v>0</v>
@@ -6339,7 +6341,7 @@
         <v>8</v>
       </c>
       <c r="C225" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D225" s="6">
         <v>2</v>
@@ -6361,7 +6363,7 @@
         <v>8</v>
       </c>
       <c r="C226" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D226" s="6">
         <v>0</v>
@@ -6383,7 +6385,7 @@
         <v>8</v>
       </c>
       <c r="C227" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D227" s="6">
         <v>0</v>
@@ -6405,7 +6407,7 @@
         <v>8</v>
       </c>
       <c r="C228" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D228" s="6">
         <v>0</v>
@@ -6427,7 +6429,7 @@
         <v>8</v>
       </c>
       <c r="C229" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D229" s="6">
         <v>0</v>
@@ -6449,7 +6451,7 @@
         <v>8</v>
       </c>
       <c r="C230" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D230" s="5">
         <v>3</v>
@@ -6471,7 +6473,7 @@
         <v>8</v>
       </c>
       <c r="C231" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D231" s="5">
         <v>2</v>
@@ -6493,7 +6495,7 @@
         <v>8</v>
       </c>
       <c r="C232" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D232" s="5">
         <v>2</v>
@@ -6515,7 +6517,7 @@
         <v>8</v>
       </c>
       <c r="C233" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D233" s="5">
         <v>0</v>
@@ -6537,7 +6539,7 @@
         <v>8</v>
       </c>
       <c r="C234" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D234" s="5">
         <v>3</v>
@@ -6559,7 +6561,7 @@
         <v>8</v>
       </c>
       <c r="C235" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D235" s="5">
         <v>0</v>
@@ -6581,7 +6583,7 @@
         <v>8</v>
       </c>
       <c r="C236" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D236" s="6">
         <v>3</v>
@@ -6603,7 +6605,7 @@
         <v>8</v>
       </c>
       <c r="C237" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D237" s="6">
         <v>2</v>
@@ -6625,7 +6627,7 @@
         <v>8</v>
       </c>
       <c r="C238" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D238" s="6">
         <v>2</v>
@@ -6647,7 +6649,7 @@
         <v>8</v>
       </c>
       <c r="C239" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D239" s="6">
         <v>2</v>
@@ -6669,7 +6671,7 @@
         <v>8</v>
       </c>
       <c r="C240" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D240" s="6">
         <v>2</v>
@@ -6691,7 +6693,7 @@
         <v>8</v>
       </c>
       <c r="C241" s="13">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D241" s="6">
         <v>2</v>

</xml_diff>